<commit_message>
音節表勘誤 pha(在p,ah) -> pah
</commit_message>
<xml_diff>
--- a/臺灣閩南語TaiwaneseCVVC入聲音節表.xlsx
+++ b/臺灣閩南語TaiwaneseCVVC入聲音節表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\UTAU-Taiwanese-Voicebank-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40DF725-8E76-490D-ADE8-A692D9C954AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0FB7BD3-54D6-4B7D-8311-4394D1185B1A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1390,10 +1390,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>pha 拍</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>pak 覆</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -2083,6 +2079,10 @@
   </si>
   <si>
     <t>臺灣閩南語TaiwaneseCVVC入聲音節表</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pah 拍</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -2758,7 +2758,7 @@
   <dimension ref="A1:U36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2781,7 +2781,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="35" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B1" s="35"/>
       <c r="C1" s="35"/>
@@ -2809,25 +2809,25 @@
         <v>0</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>134</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>2</v>
@@ -2836,28 +2836,28 @@
         <v>3</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="O2" s="22" t="s">
+        <v>312</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="R2" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>6</v>
@@ -2877,35 +2877,35 @@
         <v>135</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>154</v>
+        <v>345</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="8" t="s">
         <v>153</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="Q3" s="9" t="s">
         <v>10</v>
@@ -2929,37 +2929,37 @@
         <v>136</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="8" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I4" s="10"/>
       <c r="J4" s="9" t="s">
         <v>14</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N4" s="10"/>
       <c r="O4" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P4" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="Q4" s="9" t="s">
         <v>15</v>
@@ -3014,30 +3014,30 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="G6" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="9" t="s">
         <v>22</v>
       </c>
       <c r="K6" s="8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="M6" s="8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N6" s="10"/>
       <c r="O6" s="21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="P6" s="8" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="Q6" s="9" t="s">
         <v>23</v>
@@ -3063,31 +3063,31 @@
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="I7" s="10"/>
       <c r="J7" s="9" t="s">
         <v>27</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
       <c r="O7" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="P7" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="Q7" s="9" t="s">
         <v>28</v>
@@ -3111,16 +3111,16 @@
         <v>138</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>32</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H8" s="10"/>
       <c r="I8" s="9" t="s">
@@ -3130,7 +3130,7 @@
         <v>34</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="L8" s="15"/>
       <c r="M8" s="10"/>
@@ -3159,13 +3159,13 @@
         <v>37</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>38</v>
@@ -3174,20 +3174,20 @@
         <v>39</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="M9" s="10"/>
       <c r="N9" s="9" t="s">
         <v>40</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="P9" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Q9" s="9" t="s">
         <v>41</v>
@@ -3217,7 +3217,7 @@
       <c r="J10" s="10"/>
       <c r="K10" s="10"/>
       <c r="L10" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
@@ -3239,12 +3239,12 @@
         <v>140</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
       <c r="G11" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>46</v>
@@ -3254,26 +3254,26 @@
         <v>47</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="24" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="P11" s="25" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="Q11" s="25" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="R11" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="S11" s="9" t="s">
         <v>48</v>
@@ -3293,30 +3293,30 @@
         <v>141</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12" s="8" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>
       <c r="K12" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
       <c r="O12" s="26"/>
       <c r="P12" s="25" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="Q12" s="25" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="R12" s="10"/>
       <c r="S12" s="10"/>
@@ -3334,33 +3334,33 @@
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="8" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I13" s="10"/>
       <c r="J13" s="9" t="s">
         <v>52</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M13" s="8" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P13" s="25" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Q13" s="25" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="R13" s="10"/>
       <c r="S13" s="9" t="s">
@@ -3381,43 +3381,43 @@
         <v>142</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E14" s="10"/>
       <c r="F14" s="8" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G14" s="8" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="H14" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I14" s="10"/>
       <c r="J14" s="9" t="s">
         <v>56</v>
       </c>
       <c r="K14" s="8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="L14" s="8" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="P14" s="25" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="Q14" s="25" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="R14" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="S14" s="9" t="s">
         <v>57</v>
@@ -3444,13 +3444,13 @@
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="8" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M15" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N15" s="9" t="s">
         <v>61</v>
@@ -3475,19 +3475,19 @@
         <v>143</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>64</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>65</v>
@@ -3497,18 +3497,18 @@
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="M16" s="10"/>
       <c r="N16" s="10"/>
       <c r="O16" s="24" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q16" s="25" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="10"/>
@@ -3525,40 +3525,40 @@
         <v>144</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I17" s="10"/>
       <c r="J17" s="9" t="s">
         <v>68</v>
       </c>
       <c r="K17" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L17" s="8" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="M17" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="24" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="P17" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="Q17" s="25" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="R17" s="10"/>
       <c r="S17" s="9" t="s">
@@ -3580,7 +3580,7 @@
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
@@ -3608,7 +3608,7 @@
       <c r="E19" s="10"/>
       <c r="F19" s="10"/>
       <c r="G19" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
@@ -3616,21 +3616,21 @@
         <v>73</v>
       </c>
       <c r="K19" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L19" s="8" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="24" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="P19" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="Q19" s="25" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="R19" s="10"/>
       <c r="S19" s="9" t="s">
@@ -3652,36 +3652,36 @@
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H20" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I20" s="13"/>
       <c r="J20" s="5" t="s">
         <v>77</v>
       </c>
       <c r="K20" s="7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="L20" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="M20" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="N20" s="13"/>
       <c r="O20" s="28" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P20" s="29" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="Q20" s="29" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="R20" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="S20" s="5" t="s">
         <v>78</v>
@@ -3708,24 +3708,24 @@
         <v>81</v>
       </c>
       <c r="K21" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="L21" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M21" s="13"/>
       <c r="N21" s="13"/>
       <c r="O21" s="28" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="P21" s="29" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q21" s="29" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="R21" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="S21" s="5" t="s">
         <v>82</v>
@@ -3745,39 +3745,39 @@
         <v>145</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E22" s="13"/>
       <c r="F22" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H22" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I22" s="13"/>
       <c r="J22" s="13"/>
       <c r="K22" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="L22" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="M22" s="13"/>
       <c r="N22" s="13"/>
       <c r="O22" s="28" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="P22" s="29" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="Q22" s="29" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="R22" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="S22" s="5" t="s">
         <v>85</v>
@@ -3798,13 +3798,13 @@
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
       <c r="G23" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
       <c r="K23" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="L23" s="16"/>
       <c r="M23" s="13"/>
@@ -3853,7 +3853,7 @@
       </c>
       <c r="C25" s="13"/>
       <c r="D25" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
@@ -3867,7 +3867,7 @@
       <c r="N25" s="13"/>
       <c r="O25" s="20"/>
       <c r="P25" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q25" s="13"/>
       <c r="R25" s="13"/>
@@ -3887,31 +3887,31 @@
         <v>146</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
       <c r="G26" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H26" s="7" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="I26" s="13"/>
       <c r="J26" s="5" t="s">
         <v>93</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="L26" s="16"/>
       <c r="M26" s="13"/>
       <c r="N26" s="13"/>
       <c r="O26" s="19" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P26" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="Q26" s="5" t="s">
         <v>94</v>
@@ -3935,37 +3935,37 @@
         <v>147</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E27" s="13"/>
       <c r="F27" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="I27" s="13"/>
       <c r="J27" s="5" t="s">
         <v>98</v>
       </c>
       <c r="K27" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="L27" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="M27" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="N27" s="13"/>
       <c r="O27" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P27" s="7" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q27" s="5" t="s">
         <v>99</v>
@@ -4045,39 +4045,39 @@
         <v>148</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E30" s="13"/>
       <c r="F30" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="I30" s="13"/>
       <c r="J30" s="5" t="s">
         <v>107</v>
       </c>
       <c r="K30" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="L30" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="M30" s="13"/>
       <c r="N30" s="13"/>
       <c r="O30" s="19" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="P30" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Q30" s="5" t="s">
         <v>108</v>
       </c>
       <c r="R30" s="17" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="S30" s="5" t="s">
         <v>109</v>
@@ -4097,34 +4097,34 @@
         <v>149</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E31" s="13"/>
       <c r="F31" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="5" t="s">
         <v>112</v>
       </c>
       <c r="K31" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="L31" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="M31" s="7" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="N31" s="13"/>
       <c r="O31" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="P31" s="16"/>
       <c r="Q31" s="5" t="s">
@@ -4149,24 +4149,24 @@
         <v>150</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
       <c r="J32" s="13"/>
       <c r="K32" s="7" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="L32" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="M32" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N32" s="5" t="s">
         <v>117</v>
@@ -4198,7 +4198,7 @@
       <c r="E33" s="13"/>
       <c r="F33" s="13"/>
       <c r="G33" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="H33" s="5" t="s">
         <v>122</v>
@@ -4210,10 +4210,10 @@
       <c r="M33" s="13"/>
       <c r="N33" s="13"/>
       <c r="O33" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Q33" s="5" t="s">
         <v>123</v>
@@ -4235,35 +4235,35 @@
         <v>152</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E34" s="13"/>
       <c r="F34" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="I34" s="13"/>
       <c r="J34" s="5" t="s">
         <v>126</v>
       </c>
       <c r="K34" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M34" s="13"/>
       <c r="N34" s="13"/>
       <c r="O34" s="19" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="P34" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="Q34" s="5" t="s">
         <v>127</v>

</xml_diff>